<commit_message>
updated with unique apks only
</commit_message>
<xml_diff>
--- a/resources/data/charts.xlsx
+++ b/resources/data/charts.xlsx
@@ -2286,7 +2286,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0858922"/>
+          <c:x val="0.0858921"/>
           <c:y val="0"/>
           <c:w val="0.892901"/>
           <c:h val="0.0633182"/>
@@ -2341,9 +2341,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.110362"/>
+          <c:x val="0.116246"/>
           <c:y val="0.12131"/>
-          <c:w val="0.884638"/>
+          <c:w val="0.878754"/>
           <c:h val="0.794572"/>
         </c:manualLayout>
       </c:layout>
@@ -2517,94 +2517,94 @@
                   <c:v>1.000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1.000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>2.000000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>2.000000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
+                  <c:v>2.000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>3.000000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10">
                   <c:v>3.000000</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
+                  <c:v>3.000000</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>4.000000</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="13">
                   <c:v>4.000000</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="14">
+                  <c:v>6.000000</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>9.000000</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="16">
                   <c:v>9.000000</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="17">
                   <c:v>10.000000</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="18">
+                  <c:v>11.000000</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>12.000000</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="20">
+                  <c:v>12.000000</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>13.000000</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="22">
                   <c:v>13.000000</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>13.000000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>13.000000</c:v>
-                </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="23">
                   <c:v>14.000000</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>16.000000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>18.000000</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20.000000</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>41.000000</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>45.000000</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>51.000000</c:v>
-                </c:pt>
                 <c:pt idx="24">
-                  <c:v>54.000000</c:v>
+                  <c:v>15.000000</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>60.000000</c:v>
+                  <c:v>21.000000</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>101.000000</c:v>
+                  <c:v>27.000000</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>101.000000</c:v>
+                  <c:v>28.000000</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>121.000000</c:v>
+                  <c:v>33.000000</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>129.000000</c:v>
+                  <c:v>33.000000</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>143.000000</c:v>
+                  <c:v>58.000000</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>316.000000</c:v>
+                  <c:v>70.000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2759,8 +2759,8 @@
         <c:crossAx val="2094734552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="100"/>
-        <c:minorUnit val="50"/>
+        <c:majorUnit val="17.5"/>
+        <c:minorUnit val="8.75"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2777,9 +2777,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0899947"/>
+          <c:x val="0.0960129"/>
           <c:y val="0"/>
-          <c:w val="0.86211"/>
+          <c:w val="0.856409"/>
           <c:h val="0.0633182"/>
         </c:manualLayout>
       </c:layout>
@@ -3268,7 +3268,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0621037"/>
+          <c:x val="0.0621036"/>
           <c:y val="0"/>
           <c:w val="0.891795"/>
           <c:h val="0.0633182"/>
@@ -4313,7 +4313,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0337239"/>
+          <c:x val="0.0337238"/>
           <c:y val="0"/>
           <c:w val="0.9"/>
           <c:h val="0.0640667"/>
@@ -4361,13 +4361,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>653034</xdr:colOff>
+      <xdr:colOff>653033</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>117263</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>977900</xdr:colOff>
+      <xdr:colOff>977899</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>6087</xdr:rowOff>
     </xdr:to>
@@ -4378,7 +4378,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="9365233" y="877993"/>
-        <a:ext cx="5303268" cy="3710890"/>
+        <a:ext cx="5303267" cy="3710890"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4402,7 +4402,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1122680</xdr:colOff>
+      <xdr:colOff>1122679</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>19887</xdr:rowOff>
     </xdr:to>
@@ -4412,8 +4412,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7020813" y="1638553"/>
-        <a:ext cx="5303268" cy="3710890"/>
+        <a:off x="7020814" y="1638553"/>
+        <a:ext cx="5303266" cy="3710890"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4448,7 +4448,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="-256811" y="3849242"/>
-        <a:ext cx="5412012" cy="4034526"/>
+        <a:ext cx="5412011" cy="4034526"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4466,7 +4466,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>517651</xdr:colOff>
+      <xdr:colOff>517652</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4482,7 +4482,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6740651" y="0"/>
+        <a:off x="6740652" y="0"/>
         <a:ext cx="5120387" cy="3884423"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -4501,13 +4501,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>411733</xdr:colOff>
+      <xdr:colOff>376427</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
+      <xdr:colOff>736599</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>217932</xdr:rowOff>
     </xdr:to>
@@ -4517,8 +4517,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6634733" y="0"/>
-        <a:ext cx="5303267" cy="3884423"/>
+        <a:off x="6599427" y="0"/>
+        <a:ext cx="5338573" cy="3884423"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4552,8 +4552,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6811263" y="0"/>
-        <a:ext cx="5126737" cy="3884423"/>
+        <a:off x="6811264" y="0"/>
+        <a:ext cx="5126736" cy="3884423"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4571,13 +4571,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
+      <xdr:colOff>634999</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
+      <xdr:colOff>736599</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>245745</xdr:rowOff>
     </xdr:to>
@@ -4588,7 +4588,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="6857999" y="0"/>
-        <a:ext cx="5080002" cy="3810000"/>
+        <a:ext cx="5080001" cy="3810000"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7591,7 +7591,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -7602,7 +7602,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -7613,7 +7613,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -7624,7 +7624,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -7635,7 +7635,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -7646,7 +7646,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -7657,7 +7657,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -7668,7 +7668,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="9">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -7679,7 +7679,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="9">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -7690,7 +7690,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="9">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -7701,7 +7701,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="9">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -7712,7 +7712,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="9">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -7723,7 +7723,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="9">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -7734,7 +7734,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="9">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -7745,7 +7745,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="9">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -7756,7 +7756,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="9">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -7767,7 +7767,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="9">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -7778,7 +7778,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="9">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -7789,7 +7789,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="9">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -7800,7 +7800,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="9">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -7811,7 +7811,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="9">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -7822,7 +7822,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="9">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -7833,7 +7833,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="9">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -7844,7 +7844,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="9">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -7855,7 +7855,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="9">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -7866,7 +7866,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="9">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -7877,7 +7877,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="9">
-        <v>121</v>
+        <v>33</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -7888,7 +7888,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="9">
-        <v>129</v>
+        <v>33</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -7899,7 +7899,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="9">
-        <v>143</v>
+        <v>58</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -7910,7 +7910,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="9">
-        <v>316</v>
+        <v>70</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>

</xml_diff>